<commit_message>
added programm for preparing data
</commit_message>
<xml_diff>
--- a/подсистема обработки ТИ из ОИК/Описание.xlsx
+++ b/подсистема обработки ТИ из ОИК/Описание.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t>Address</t>
   </si>
@@ -121,13 +121,166 @@
   </si>
   <si>
     <t>Сначала проходим по всем state. Ищем соответствие. Сначала проверяется состояние сетевых элементов с наиболее высоким напряжением (550-750 кВ) и состояние генераторов с наибольшей номинальной мощностью (300 МВт и выше). Затем более низкое напряжение (220-330 кВ) и мощность (150-300 МВт). И самое низкое напряжение (110 кВ) и мощность (ниже 150 МВт). На каждом шаге отсеивается часть схем. Остается наиболее похожая. Далее сравниваются все остальные значения (напряжение, перетоки, вырабатываемая мощность, токи). При чем при сравнении должны использоваться весовые коэффициенты в зависимости от базового напряжения узла и номинальной мощности генератора. Остается одна наиболее схожая схема.</t>
+  </si>
+  <si>
+    <t>FirstNode</t>
+  </si>
+  <si>
+    <t>LastNode</t>
+  </si>
+  <si>
+    <t>NominalVoltage</t>
+  </si>
+  <si>
+    <t>ActivePowerAtFirst</t>
+  </si>
+  <si>
+    <t>ActivePowerInTheEnd</t>
+  </si>
+  <si>
+    <t>ReactivePowerAtFirst</t>
+  </si>
+  <si>
+    <t>ReactivePowerInTheEnd</t>
+  </si>
+  <si>
+    <t>CurrentAtFirst</t>
+  </si>
+  <si>
+    <t>CurrentInTheEnd</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>CalculatedVoltage</t>
+  </si>
+  <si>
+    <t>ActiveLoad</t>
+  </si>
+  <si>
+    <t>ReactiveLoad</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Transformer</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>ConnectionNode</t>
+  </si>
+  <si>
+    <t>NominalActivePower</t>
+  </si>
+  <si>
+    <t>Edges</t>
+  </si>
+  <si>
+    <t>LineSegments</t>
+  </si>
+  <si>
+    <t>Transformers</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>Telemetry</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Types:</t>
+  </si>
+  <si>
+    <t>NetworkElementState</t>
+  </si>
+  <si>
+    <t>GeneratorState</t>
+  </si>
+  <si>
+    <t>NodeVoltage</t>
+  </si>
+  <si>
+    <t>NodeActiveLoad</t>
+  </si>
+  <si>
+    <t>NodeReactiveLoad</t>
+  </si>
+  <si>
+    <t>LineSegmentActivePowerAtFirst</t>
+  </si>
+  <si>
+    <t>LineSegmentActivePowerInTheEnd</t>
+  </si>
+  <si>
+    <t>LineSegmentReactivePowerAtFirst</t>
+  </si>
+  <si>
+    <t>LineSegmentReactivePowerInTheEnd</t>
+  </si>
+  <si>
+    <t>LineSegmentCurrentAtFirst</t>
+  </si>
+  <si>
+    <t>LineSegmentCurrentInTheEnd</t>
+  </si>
+  <si>
+    <t>TransformerActivePower</t>
+  </si>
+  <si>
+    <t>TransformerReactivePower</t>
+  </si>
+  <si>
+    <t>TransformerCurrent</t>
+  </si>
+  <si>
+    <t>GeneratorActivePower</t>
+  </si>
+  <si>
+    <t>GeneratorReactivePower</t>
+  </si>
+  <si>
+    <t>:Parametr</t>
+  </si>
+  <si>
+    <t>NetworkElementData</t>
+  </si>
+  <si>
+    <t>GeneratorData</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>ControlParametr</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>"type of object"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,16 +325,90 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE3FD83"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -274,11 +501,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -340,6 +589,47 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,6 +637,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE3FD83"/>
+      <color rgb="FFCCFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -621,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:AG39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,12 +935,24 @@
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="12.21875" customWidth="1"/>
     <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" customWidth="1"/>
-    <col min="15" max="15" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.33203125" customWidth="1"/>
+    <col min="23" max="23" width="11.5546875" customWidth="1"/>
+    <col min="24" max="24" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5546875" customWidth="1"/>
+    <col min="29" max="29" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -661,17 +969,56 @@
         <v>30</v>
       </c>
       <c r="J1" s="15"/>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="29" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="S1" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="V1" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="X1" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB1" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC1" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE1" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -695,16 +1042,46 @@
       </c>
       <c r="J2" s="15"/>
       <c r="N2" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -721,17 +1098,47 @@
         <v>25</v>
       </c>
       <c r="J3" s="15"/>
-      <c r="N3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N3" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -754,17 +1161,35 @@
         <v>16</v>
       </c>
       <c r="J4" s="15"/>
-      <c r="N4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N4" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="X4" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -781,15 +1206,29 @@
         <v>25</v>
       </c>
       <c r="J5" s="15"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="X5" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y5" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -812,15 +1251,26 @@
         <v>24</v>
       </c>
       <c r="J6" s="15"/>
-      <c r="N6" s="4"/>
+      <c r="N6" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="O6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="X6" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y6" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -837,12 +1287,23 @@
         <v>27</v>
       </c>
       <c r="J7" s="15"/>
-      <c r="N7" s="4"/>
+      <c r="N7" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="O7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="X7" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y7" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -862,12 +1323,23 @@
         <v>13</v>
       </c>
       <c r="J8" s="15"/>
-      <c r="N8" s="4"/>
+      <c r="N8" s="35" t="s">
+        <v>47</v>
+      </c>
       <c r="O8" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="X8" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y8" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -886,10 +1358,16 @@
       <c r="J9" s="15"/>
       <c r="N9" s="4"/>
       <c r="O9" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="X9" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y9" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -906,8 +1384,17 @@
         <v>19</v>
       </c>
       <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="X10" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y10" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -924,8 +1411,17 @@
         <v>20</v>
       </c>
       <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O11" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="X11" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y11" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -942,8 +1438,14 @@
         <v>21</v>
       </c>
       <c r="J12" s="15"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="X12" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y12" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -960,8 +1462,14 @@
         <v>22</v>
       </c>
       <c r="J13" s="15"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="X13" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y13" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -978,8 +1486,14 @@
         <v>23</v>
       </c>
       <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="X14" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y14" s="41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -996,8 +1510,17 @@
         <v>15</v>
       </c>
       <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="X15" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y15" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1010,6 +1533,12 @@
       </c>
       <c r="F16" s="2"/>
       <c r="J16" s="15"/>
+      <c r="X16" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y16" s="42" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>

</xml_diff>